<commit_message>
remake the npc pos
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/PeopleChess.xlsx
+++ b/ConfigData/Xlsx/PeopleChess.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="131">
   <si>
     <t>塞尼斯</t>
   </si>
@@ -276,149 +276,208 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>116</t>
+  </si>
+  <si>
+    <t>117</t>
+  </si>
+  <si>
+    <t>118</t>
+  </si>
+  <si>
+    <t>119</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>121</t>
+  </si>
+  <si>
+    <t>122</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>124</t>
+  </si>
+  <si>
+    <t>125</t>
+  </si>
+  <si>
+    <t>126</t>
+  </si>
+  <si>
+    <t>127</t>
+  </si>
+  <si>
+    <t>137</t>
+  </si>
+  <si>
+    <t>138</t>
+  </si>
+  <si>
+    <t>139</t>
+  </si>
+  <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>141</t>
+  </si>
+  <si>
+    <t>142</t>
+  </si>
+  <si>
+    <t>143</t>
+  </si>
+  <si>
+    <t>144</t>
+  </si>
+  <si>
+    <t>145</t>
+  </si>
+  <si>
+    <t>146</t>
+  </si>
+  <si>
+    <t>13010002</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>13010003,13010002</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>100,30</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>13010003,13010004</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>70,100</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>100</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>101</t>
-  </si>
-  <si>
-    <t>102</t>
-  </si>
-  <si>
-    <t>103</t>
-  </si>
-  <si>
-    <t>104</t>
-  </si>
-  <si>
-    <t>105</t>
-  </si>
-  <si>
-    <t>106</t>
-  </si>
-  <si>
-    <t>107</t>
-  </si>
-  <si>
-    <t>108</t>
-  </si>
-  <si>
-    <t>109</t>
-  </si>
-  <si>
-    <t>110</t>
-  </si>
-  <si>
-    <t>111</t>
-  </si>
-  <si>
-    <t>112</t>
-  </si>
-  <si>
-    <t>113</t>
-  </si>
-  <si>
-    <t>114</t>
-  </si>
-  <si>
-    <t>115</t>
-  </si>
-  <si>
-    <t>116</t>
-  </si>
-  <si>
-    <t>117</t>
-  </si>
-  <si>
-    <t>118</t>
-  </si>
-  <si>
-    <t>119</t>
-  </si>
-  <si>
-    <t>120</t>
-  </si>
-  <si>
-    <t>121</t>
-  </si>
-  <si>
-    <t>122</t>
-  </si>
-  <si>
-    <t>123</t>
-  </si>
-  <si>
-    <t>124</t>
-  </si>
-  <si>
-    <t>125</t>
-  </si>
-  <si>
-    <t>126</t>
-  </si>
-  <si>
-    <t>127</t>
-  </si>
-  <si>
-    <t>128</t>
-  </si>
-  <si>
-    <t>129</t>
-  </si>
-  <si>
-    <t>130</t>
-  </si>
-  <si>
-    <t>131</t>
-  </si>
-  <si>
-    <t>132</t>
-  </si>
-  <si>
-    <t>133</t>
-  </si>
-  <si>
-    <t>134</t>
-  </si>
-  <si>
-    <t>135</t>
-  </si>
-  <si>
-    <t>136</t>
-  </si>
-  <si>
-    <t>137</t>
-  </si>
-  <si>
-    <t>138</t>
-  </si>
-  <si>
-    <t>139</t>
-  </si>
-  <si>
-    <t>140</t>
-  </si>
-  <si>
-    <t>141</t>
-  </si>
-  <si>
-    <t>142</t>
-  </si>
-  <si>
-    <t>143</t>
-  </si>
-  <si>
-    <t>144</t>
-  </si>
-  <si>
-    <t>145</t>
-  </si>
-  <si>
-    <t>146</t>
-  </si>
-  <si>
-    <t>13010002,13010003</t>
+    <t>13010004,13010009</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>70,130</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>13010004,0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>50,100</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>13010008,13010005,0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>120,40,80</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>13010203,0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>100,100</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>13010202,0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>13010102</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>13010103,13010104</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>13010106,13010110,0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>50,80,100</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>13010108,13010109</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>13010107</t>
+  </si>
+  <si>
+    <t>13010104,0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>65,100</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>13010102,13010106,0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>80,80,60</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>13010206</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>13010208,13010209,13010204</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>100,100,100</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>13010207,0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>13010202</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>13010202,13010203</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>60,120</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>80,100,0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>13010205,13010209,0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>13010208</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1150,7 +1209,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="41">
+  <dxfs count="17">
     <dxf>
       <font>
         <b val="0"/>
@@ -1169,7 +1228,6 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -1241,326 +1299,6 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1578,6 +1316,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -1699,6 +1438,62 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1781,18 +1576,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表2_4" displayName="表2_4" ref="A3:F51" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39" tableBorderDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表2_4" displayName="表2_4" ref="A3:F51" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" tableBorderDxfId="6">
   <autoFilter ref="A3:F51"/>
   <sortState ref="A4:F50">
     <sortCondition ref="A3:A50"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="Id" dataDxfId="37"/>
-    <tableColumn id="2" name="~Name" dataDxfId="36"/>
-    <tableColumn id="7" name="BornSceneId" dataDxfId="0"/>
+    <tableColumn id="1" name="Id" dataDxfId="5"/>
+    <tableColumn id="2" name="~Name" dataDxfId="4"/>
+    <tableColumn id="7" name="BornSceneId" dataDxfId="3"/>
     <tableColumn id="4" name="BornSceneBeginer" dataDxfId="2"/>
     <tableColumn id="3" name="BornSceneChecker" dataDxfId="1"/>
-    <tableColumn id="8" name="BindQuest" dataDxfId="35"/>
+    <tableColumn id="8" name="BindQuest" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2125,14 +1920,14 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.25" customWidth="1"/>
-    <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="9.5" customWidth="1"/>
+    <col min="3" max="3" width="23.25" customWidth="1"/>
+    <col min="4" max="4" width="6.625" customWidth="1"/>
     <col min="5" max="5" width="19.125" customWidth="1"/>
     <col min="6" max="6" width="9.75" customWidth="1"/>
   </cols>
@@ -2205,7 +2000,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>121</v>
+        <v>96</v>
       </c>
       <c r="D4" s="3">
         <v>30</v>
@@ -2224,14 +2019,14 @@
       <c r="B5" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="9">
-        <v>13010003</v>
+      <c r="C5" s="9" t="s">
+        <v>97</v>
       </c>
       <c r="D5" s="3">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>74</v>
+        <v>98</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>60</v>
@@ -2244,14 +2039,14 @@
       <c r="B6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="9">
-        <v>13010004</v>
+      <c r="C6" s="9" t="s">
+        <v>99</v>
       </c>
       <c r="D6" s="3">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>62</v>
@@ -2268,10 +2063,10 @@
         <v>13010007</v>
       </c>
       <c r="D7" s="3">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>63</v>
@@ -2284,14 +2079,14 @@
       <c r="B8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="9">
-        <v>13010009</v>
+      <c r="C8" s="9" t="s">
+        <v>102</v>
       </c>
       <c r="D8" s="3">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>61</v>
@@ -2304,14 +2099,14 @@
       <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="9">
-        <v>13010008</v>
+      <c r="C9" s="9" t="s">
+        <v>106</v>
       </c>
       <c r="D9" s="3">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>78</v>
+        <v>107</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>64</v>
@@ -2324,12 +2119,14 @@
       <c r="B10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="9"/>
+      <c r="C10" s="9" t="s">
+        <v>104</v>
+      </c>
       <c r="D10" s="3">
         <v>36</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="F10" s="3"/>
     </row>
@@ -2340,14 +2137,14 @@
       <c r="B11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="9">
-        <v>13010203</v>
+      <c r="C11" s="9" t="s">
+        <v>108</v>
       </c>
       <c r="D11" s="3">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>80</v>
+        <v>109</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>65</v>
@@ -2360,14 +2157,14 @@
       <c r="B12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="9">
-        <v>13010202</v>
+      <c r="C12" s="9" t="s">
+        <v>110</v>
       </c>
       <c r="D12" s="3">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>81</v>
+        <v>109</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>66</v>
@@ -2380,14 +2177,14 @@
       <c r="B13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="9">
-        <v>13010203</v>
+      <c r="C13" s="9" t="s">
+        <v>108</v>
       </c>
       <c r="D13" s="3">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>82</v>
+        <v>105</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>67</v>
@@ -2400,14 +2197,14 @@
       <c r="B14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="9">
-        <v>13010103</v>
+      <c r="C14" s="9" t="s">
+        <v>121</v>
       </c>
       <c r="D14" s="3">
         <v>40</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>83</v>
+        <v>101</v>
       </c>
       <c r="F14" s="3"/>
     </row>
@@ -2418,12 +2215,14 @@
       <c r="B15" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="9"/>
+      <c r="C15" s="9" t="s">
+        <v>122</v>
+      </c>
       <c r="D15" s="3">
-        <v>41</v>
+        <v>10</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>84</v>
+        <v>123</v>
       </c>
       <c r="F15" s="3"/>
     </row>
@@ -2434,12 +2233,14 @@
       <c r="B16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="9"/>
+      <c r="C16" s="9" t="s">
+        <v>124</v>
+      </c>
       <c r="D16" s="3">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>85</v>
+        <v>103</v>
       </c>
       <c r="F16" s="3"/>
     </row>
@@ -2450,14 +2251,14 @@
       <c r="B17" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="9">
-        <v>13010107</v>
+      <c r="C17" s="9" t="s">
+        <v>125</v>
       </c>
       <c r="D17" s="3">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="F17" s="3"/>
     </row>
@@ -2468,14 +2269,14 @@
       <c r="B18" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="9">
-        <v>13010202</v>
+      <c r="C18" s="9" t="s">
+        <v>126</v>
       </c>
       <c r="D18" s="3">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>87</v>
+        <v>127</v>
       </c>
       <c r="F18" s="3"/>
     </row>
@@ -2486,14 +2287,14 @@
       <c r="B19" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="9">
-        <v>13010205</v>
+      <c r="C19" s="9" t="s">
+        <v>129</v>
       </c>
       <c r="D19" s="3">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>88</v>
+        <v>128</v>
       </c>
       <c r="F19" s="3"/>
     </row>
@@ -2504,12 +2305,14 @@
       <c r="B20" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="9"/>
+      <c r="C20" s="9" t="s">
+        <v>130</v>
+      </c>
       <c r="D20" s="3">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="F20" s="3"/>
     </row>
@@ -2520,14 +2323,12 @@
       <c r="B21" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="9">
-        <v>13010102</v>
-      </c>
+      <c r="C21" s="9"/>
       <c r="D21" s="3">
         <v>47</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="F21" s="3"/>
     </row>
@@ -2543,7 +2344,7 @@
         <v>48</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="F22" s="3"/>
     </row>
@@ -2554,14 +2355,12 @@
       <c r="B23" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="9">
-        <v>13010106</v>
-      </c>
+      <c r="C23" s="9"/>
       <c r="D23" s="3">
         <v>49</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="F23" s="3"/>
     </row>
@@ -2577,7 +2376,7 @@
         <v>50</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="F24" s="3"/>
     </row>
@@ -2588,14 +2387,12 @@
       <c r="B25" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="9">
-        <v>13010204</v>
-      </c>
+      <c r="C25" s="9"/>
       <c r="D25" s="3">
         <v>51</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="F25" s="3"/>
     </row>
@@ -2606,14 +2403,12 @@
       <c r="B26" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="9">
-        <v>13010204</v>
-      </c>
+      <c r="C26" s="9"/>
       <c r="D26" s="3">
         <v>52</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="F26" s="3"/>
     </row>
@@ -2624,14 +2419,12 @@
       <c r="B27" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="9">
-        <v>13010102</v>
-      </c>
+      <c r="C27" s="9"/>
       <c r="D27" s="3">
         <v>53</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="F27" s="3"/>
     </row>
@@ -2647,7 +2440,7 @@
         <v>54</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="F28" s="3"/>
     </row>
@@ -2658,14 +2451,12 @@
       <c r="B29" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="9">
-        <v>13010105</v>
-      </c>
+      <c r="C29" s="9"/>
       <c r="D29" s="3">
         <v>55</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="F29" s="3"/>
     </row>
@@ -2676,14 +2467,12 @@
       <c r="B30" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="9">
-        <v>13010105</v>
-      </c>
+      <c r="C30" s="9"/>
       <c r="D30" s="3">
         <v>56</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="F30" s="3"/>
     </row>
@@ -2699,7 +2488,7 @@
         <v>57</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="F31" s="3"/>
     </row>
@@ -2715,7 +2504,7 @@
         <v>58</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="F32" s="3"/>
     </row>
@@ -2726,14 +2515,14 @@
       <c r="B33" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="9">
-        <v>13010108</v>
+      <c r="C33" s="9" t="s">
+        <v>111</v>
       </c>
       <c r="D33" s="3">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F33" s="3"/>
     </row>
@@ -2744,14 +2533,14 @@
       <c r="B34" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="9">
-        <v>13010103</v>
+      <c r="C34" s="9" t="s">
+        <v>111</v>
       </c>
       <c r="D34" s="3">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F34" s="3"/>
     </row>
@@ -2762,12 +2551,14 @@
       <c r="B35" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C35" s="9"/>
+      <c r="C35" s="9" t="s">
+        <v>112</v>
+      </c>
       <c r="D35" s="3">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="F35" s="3"/>
     </row>
@@ -2778,14 +2569,14 @@
       <c r="B36" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C36" s="9">
-        <v>13010208</v>
+      <c r="C36" s="9" t="s">
+        <v>112</v>
       </c>
       <c r="D36" s="3">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="F36" s="3"/>
     </row>
@@ -2796,14 +2587,14 @@
       <c r="B37" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C37" s="9">
-        <v>13010108</v>
+      <c r="C37" s="9" t="s">
+        <v>113</v>
       </c>
       <c r="D37" s="3">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="F37" s="3"/>
     </row>
@@ -2814,14 +2605,14 @@
       <c r="B38" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C38" s="9">
-        <v>13010104</v>
+      <c r="C38" s="9" t="s">
+        <v>115</v>
       </c>
       <c r="D38" s="3">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="F38" s="3"/>
     </row>
@@ -2832,14 +2623,14 @@
       <c r="B39" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C39" s="9">
-        <v>13010209</v>
+      <c r="C39" s="9" t="s">
+        <v>119</v>
       </c>
       <c r="D39" s="3">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="F39" s="3"/>
     </row>
@@ -2850,14 +2641,14 @@
       <c r="B40" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C40" s="9">
-        <v>13010205</v>
+      <c r="C40" s="9" t="s">
+        <v>117</v>
       </c>
       <c r="D40" s="3">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="F40" s="3"/>
     </row>
@@ -2868,12 +2659,14 @@
       <c r="B41" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C41" s="9"/>
+      <c r="C41" s="9" t="s">
+        <v>116</v>
+      </c>
       <c r="D41" s="3">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="F41" s="3"/>
     </row>
@@ -2889,7 +2682,7 @@
         <v>68</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="F42" s="3"/>
     </row>
@@ -2900,14 +2693,12 @@
       <c r="B43" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C43" s="9">
-        <v>13010109</v>
-      </c>
+      <c r="C43" s="9"/>
       <c r="D43" s="3">
         <v>69</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="F43" s="3"/>
     </row>
@@ -2918,14 +2709,12 @@
       <c r="B44" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C44" s="9">
-        <v>13010207</v>
-      </c>
+      <c r="C44" s="9"/>
       <c r="D44" s="3">
         <v>70</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
       <c r="F44" s="3"/>
     </row>
@@ -2936,14 +2725,12 @@
       <c r="B45" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C45" s="9">
-        <v>13010209</v>
-      </c>
+      <c r="C45" s="9"/>
       <c r="D45" s="3">
         <v>71</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="F45" s="3"/>
     </row>
@@ -2954,14 +2741,12 @@
       <c r="B46" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C46" s="9">
-        <v>13010206</v>
-      </c>
+      <c r="C46" s="9"/>
       <c r="D46" s="3">
         <v>72</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="F46" s="3"/>
     </row>
@@ -2977,7 +2762,7 @@
         <v>73</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>116</v>
+        <v>91</v>
       </c>
       <c r="F47" s="7"/>
     </row>
@@ -2993,7 +2778,7 @@
         <v>74</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>117</v>
+        <v>92</v>
       </c>
       <c r="F48" s="3"/>
     </row>
@@ -3004,14 +2789,12 @@
       <c r="B49" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C49" s="9">
-        <v>13010110</v>
-      </c>
+      <c r="C49" s="9"/>
       <c r="D49" s="3">
         <v>75</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>118</v>
+        <v>93</v>
       </c>
       <c r="F49" s="3"/>
     </row>
@@ -3027,7 +2810,7 @@
         <v>76</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>119</v>
+        <v>94</v>
       </c>
       <c r="F50" s="3"/>
     </row>
@@ -3043,49 +2826,49 @@
         <v>77</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="F51" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="F5">
-    <cfRule type="containsBlanks" dxfId="10" priority="8">
+    <cfRule type="containsBlanks" dxfId="16" priority="8">
       <formula>LEN(TRIM(F5))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="containsBlanks" dxfId="9" priority="7">
+    <cfRule type="containsBlanks" dxfId="15" priority="7">
       <formula>LEN(TRIM(F8))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="containsBlanks" dxfId="8" priority="6">
+    <cfRule type="containsBlanks" dxfId="14" priority="6">
       <formula>LEN(TRIM(F6))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
-    <cfRule type="containsBlanks" dxfId="7" priority="5">
+    <cfRule type="containsBlanks" dxfId="13" priority="5">
       <formula>LEN(TRIM(F7))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="containsBlanks" dxfId="6" priority="4">
+    <cfRule type="containsBlanks" dxfId="12" priority="4">
       <formula>LEN(TRIM(F9))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11">
-    <cfRule type="containsBlanks" dxfId="5" priority="3">
+    <cfRule type="containsBlanks" dxfId="11" priority="3">
       <formula>LEN(TRIM(F11))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12">
-    <cfRule type="containsBlanks" dxfId="4" priority="2">
+    <cfRule type="containsBlanks" dxfId="10" priority="2">
       <formula>LEN(TRIM(F12))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13">
-    <cfRule type="containsBlanks" dxfId="3" priority="1">
+    <cfRule type="containsBlanks" dxfId="9" priority="1">
       <formula>LEN(TRIM(F13))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
compele the npc dialog event
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/PeopleChess.xlsx
+++ b/ConfigData/Xlsx/PeopleChess.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="132">
   <si>
     <t>塞尼斯</t>
   </si>
@@ -221,263 +221,269 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>npcsaibasi</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>npcaolai</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>npckedi</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>npcweia</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>npcbeilukai</t>
+  </si>
+  <si>
+    <t>npcleiluo</t>
+  </si>
+  <si>
+    <t>npcbaludi</t>
+  </si>
+  <si>
+    <t>~Name</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>初始场景判定子</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>BornSceneChecker</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>BornSceneBeginer</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>初始场景初始子</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>100,100</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>116</t>
+  </si>
+  <si>
+    <t>117</t>
+  </si>
+  <si>
+    <t>118</t>
+  </si>
+  <si>
+    <t>119</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>121</t>
+  </si>
+  <si>
+    <t>122</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>124</t>
+  </si>
+  <si>
+    <t>125</t>
+  </si>
+  <si>
+    <t>126</t>
+  </si>
+  <si>
+    <t>127</t>
+  </si>
+  <si>
+    <t>137</t>
+  </si>
+  <si>
+    <t>138</t>
+  </si>
+  <si>
+    <t>139</t>
+  </si>
+  <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>141</t>
+  </si>
+  <si>
+    <t>142</t>
+  </si>
+  <si>
+    <t>143</t>
+  </si>
+  <si>
+    <t>144</t>
+  </si>
+  <si>
+    <t>145</t>
+  </si>
+  <si>
+    <t>146</t>
+  </si>
+  <si>
+    <t>13010002</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>13010003,13010002</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>100,30</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>13010003,13010004</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>70,100</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>100</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>13010004,13010009</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>70,130</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>13010004,0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>50,100</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>13010008,13010005,0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>120,40,80</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>13010203,0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>100,100</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>13010202,0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>13010102</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>13010103,13010104</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>13010106,13010110,0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>50,80,100</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>13010108,13010109</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>13010107</t>
+  </si>
+  <si>
+    <t>13010104,0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>65,100</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>13010102,13010106,0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>80,80,60</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>13010206</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>13010208,13010209,13010204</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>100,100,100</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>13010207,0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>13010202</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>13010202,13010203</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>60,120</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>80,100,0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>13010205,13010209,0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>13010208</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>npcsainisi</t>
-  </si>
-  <si>
-    <t>npcsaibasi</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>npcaolai</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>npckedi</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>npcweia</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>npcmilanda</t>
-  </si>
-  <si>
-    <t>npcbeilukai</t>
-  </si>
-  <si>
-    <t>npcleiluo</t>
-  </si>
-  <si>
-    <t>npcbaludi</t>
-  </si>
-  <si>
-    <t>~Name</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>初始场景判定子</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>BornSceneChecker</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>BornSceneBeginer</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>初始场景初始子</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>100,100</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>116</t>
-  </si>
-  <si>
-    <t>117</t>
-  </si>
-  <si>
-    <t>118</t>
-  </si>
-  <si>
-    <t>119</t>
-  </si>
-  <si>
-    <t>120</t>
-  </si>
-  <si>
-    <t>121</t>
-  </si>
-  <si>
-    <t>122</t>
-  </si>
-  <si>
-    <t>123</t>
-  </si>
-  <si>
-    <t>124</t>
-  </si>
-  <si>
-    <t>125</t>
-  </si>
-  <si>
-    <t>126</t>
-  </si>
-  <si>
-    <t>127</t>
-  </si>
-  <si>
-    <t>137</t>
-  </si>
-  <si>
-    <t>138</t>
-  </si>
-  <si>
-    <t>139</t>
-  </si>
-  <si>
-    <t>140</t>
-  </si>
-  <si>
-    <t>141</t>
-  </si>
-  <si>
-    <t>142</t>
-  </si>
-  <si>
-    <t>143</t>
-  </si>
-  <si>
-    <t>144</t>
-  </si>
-  <si>
-    <t>145</t>
-  </si>
-  <si>
-    <t>146</t>
-  </si>
-  <si>
-    <t>13010002</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>13010003,13010002</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>100,30</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>13010003,13010004</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>70,100</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>100</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>13010004,13010009</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>70,130</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>13010004,0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>50,100</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>13010008,13010005,0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>120,40,80</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>13010203,0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>100,100</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>13010202,0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>13010102</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>13010103,13010104</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>13010106,13010110,0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>50,80,100</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>13010108,13010109</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>13010107</t>
-  </si>
-  <si>
-    <t>13010104,0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>65,100</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>13010102,13010106,0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>80,80,60</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>13010206</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>13010208,13010209,13010204</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>100,100,100</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>13010207,0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>13010202</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>13010202,13010203</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>60,120</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>80,100,0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>13010205,13010209,0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>13010208</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>npcgailu</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1130,7 +1136,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1162,6 +1168,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="21" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1920,7 +1929,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1943,10 +1952,10 @@
         <v>54</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>56</v>
@@ -1977,16 +1986,16 @@
         <v>39</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>55</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>58</v>
@@ -2000,16 +2009,16 @@
         <v>0</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D4" s="3">
         <v>30</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>59</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
@@ -2020,16 +2029,16 @@
         <v>43</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D5" s="3">
         <v>0</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
@@ -2040,16 +2049,16 @@
         <v>1</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D6" s="3">
         <v>20</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>62</v>
+        <v>98</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
@@ -2066,10 +2075,10 @@
         <v>0</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>63</v>
+        <v>99</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
@@ -2080,16 +2089,16 @@
         <v>3</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D8" s="3">
         <v>50</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>61</v>
+        <v>101</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
@@ -2100,16 +2109,16 @@
         <v>4</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D9" s="3">
         <v>15</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>64</v>
+        <v>105</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
@@ -2120,15 +2129,17 @@
         <v>5</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D10" s="3">
         <v>36</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="F10" s="3"/>
+        <v>103</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11">
@@ -2138,16 +2149,16 @@
         <v>6</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D11" s="3">
         <v>15</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
@@ -2158,16 +2169,16 @@
         <v>7</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D12" s="3">
         <v>45</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
@@ -2178,16 +2189,16 @@
         <v>8</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D13" s="3">
         <v>70</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
@@ -2198,13 +2209,13 @@
         <v>9</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D14" s="3">
         <v>40</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F14" s="3"/>
     </row>
@@ -2216,13 +2227,13 @@
         <v>10</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D15" s="3">
         <v>10</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F15" s="3"/>
     </row>
@@ -2234,13 +2245,13 @@
         <v>11</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D16" s="3">
         <v>60</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F16" s="3"/>
     </row>
@@ -2252,13 +2263,13 @@
         <v>41</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D17" s="3">
         <v>10</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F17" s="3"/>
     </row>
@@ -2270,13 +2281,13 @@
         <v>42</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D18" s="3">
         <v>45</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F18" s="3"/>
     </row>
@@ -2288,13 +2299,13 @@
         <v>51</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D19" s="3">
         <v>60</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F19" s="3"/>
     </row>
@@ -2306,13 +2317,13 @@
         <v>52</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D20" s="3">
         <v>20</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F20" s="3"/>
     </row>
@@ -2328,7 +2339,7 @@
         <v>47</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F21" s="3"/>
     </row>
@@ -2344,7 +2355,7 @@
         <v>48</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F22" s="3"/>
     </row>
@@ -2360,7 +2371,7 @@
         <v>49</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F23" s="3"/>
     </row>
@@ -2376,7 +2387,7 @@
         <v>50</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F24" s="3"/>
     </row>
@@ -2392,7 +2403,7 @@
         <v>51</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F25" s="3"/>
     </row>
@@ -2408,7 +2419,7 @@
         <v>52</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F26" s="3"/>
     </row>
@@ -2424,7 +2435,7 @@
         <v>53</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F27" s="3"/>
     </row>
@@ -2440,7 +2451,7 @@
         <v>54</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F28" s="3"/>
     </row>
@@ -2456,7 +2467,7 @@
         <v>55</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F29" s="3"/>
     </row>
@@ -2472,7 +2483,7 @@
         <v>56</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F30" s="3"/>
     </row>
@@ -2488,7 +2499,7 @@
         <v>57</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F31" s="3"/>
     </row>
@@ -2504,7 +2515,7 @@
         <v>58</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F32" s="3"/>
     </row>
@@ -2516,13 +2527,13 @@
         <v>23</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D33" s="3">
         <v>15</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F33" s="3"/>
     </row>
@@ -2534,13 +2545,13 @@
         <v>24</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D34" s="3">
         <v>15</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F34" s="3"/>
     </row>
@@ -2552,13 +2563,13 @@
         <v>25</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D35" s="3">
         <v>35</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F35" s="3"/>
     </row>
@@ -2570,13 +2581,13 @@
         <v>26</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D36" s="3">
         <v>65</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F36" s="3"/>
     </row>
@@ -2588,13 +2599,13 @@
         <v>27</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D37" s="3">
         <v>30</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F37" s="3"/>
     </row>
@@ -2606,13 +2617,13 @@
         <v>28</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D38" s="3">
         <v>0</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F38" s="3"/>
     </row>
@@ -2624,13 +2635,13 @@
         <v>29</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D39" s="3">
         <v>40</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F39" s="3"/>
     </row>
@@ -2642,13 +2653,13 @@
         <v>30</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D40" s="3">
         <v>35</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F40" s="3"/>
     </row>
@@ -2660,13 +2671,13 @@
         <v>44</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D41" s="3">
         <v>0</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F41" s="3"/>
     </row>
@@ -2682,7 +2693,7 @@
         <v>68</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F42" s="3"/>
     </row>
@@ -2698,7 +2709,7 @@
         <v>69</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F43" s="3"/>
     </row>
@@ -2714,7 +2725,7 @@
         <v>70</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F44" s="3"/>
     </row>
@@ -2730,7 +2741,7 @@
         <v>71</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F45" s="3"/>
     </row>
@@ -2746,7 +2757,7 @@
         <v>72</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F46" s="3"/>
     </row>
@@ -2762,7 +2773,7 @@
         <v>73</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F47" s="7"/>
     </row>
@@ -2778,7 +2789,7 @@
         <v>74</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F48" s="3"/>
     </row>
@@ -2794,7 +2805,7 @@
         <v>75</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F49" s="3"/>
     </row>
@@ -2810,7 +2821,7 @@
         <v>76</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F50" s="3"/>
     </row>
@@ -2826,7 +2837,7 @@
         <v>77</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F51" s="3"/>
     </row>

</xml_diff>